<commit_message>
Xong sign in và xử lý ngày
</commit_message>
<xml_diff>
--- a/docs/Bug/VHung.xlsx
+++ b/docs/Bug/VHung.xlsx
@@ -1,45 +1,101 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\bigdata\docs\Bug\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E91DB-BF66-4B65-8E9F-26451F7B945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Tác vụ</t>
+  </si>
+  <si>
+    <t>Tác vụ con</t>
+  </si>
+  <si>
+    <t>Hàm/Đối tượng</t>
+  </si>
+  <si>
+    <t>Lỗi/Biểu hiện</t>
+  </si>
+  <si>
+    <t>Nguyên nhân</t>
+  </si>
+  <si>
+    <t>Giải pháp</t>
+  </si>
+  <si>
+    <t>Đã thử</t>
+  </si>
+  <si>
+    <t>Tiến độ</t>
+  </si>
+  <si>
+    <t>Crawl</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>sign in</t>
+  </si>
+  <si>
+    <t>Không đăng nhập được</t>
+  </si>
+  <si>
+    <t>sau khi nhập tk mk thì nó điều hướng đến trang account.google
+Nguyên nhân rõ hơn là có 2 button có type là submit và cái soup chọn cái sign in with google</t>
+  </si>
+  <si>
+    <t>Bắt cái cookie cuối cùng
+Chọn đúng button sau</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Ngày</t>
+  </si>
+  <si>
+    <t>28/10/2025</t>
+  </si>
+  <si>
+    <t>Tổng thời gian fix</t>
+  </si>
+  <si>
+    <t>4 giờ</t>
+  </si>
+  <si>
+    <t>Kinh nghiệm rút ra</t>
+  </si>
+  <si>
+    <t>Kiểm tra kĩ CSS selector</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -72,6 +128,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,66 +460,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Tác vụ</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Tác vụ con</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Hàm/Đối tượng</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Lỗi/Biểu hiện</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Nguyên nhân</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Giải pháp</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Đã thử</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Tiến độ</v>
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
-        <v>Crawl</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Đăng nhập</v>
-      </c>
-      <c r="C2" t="str">
-        <v>sign in</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Không đăng nhập được</v>
-      </c>
-      <c r="E2" t="str" xml:space="preserve">
-        <v xml:space="preserve">sau khi nhập tk mk thì nó điều hướng đến trang account.google
-Nguyên nhân rõ hơn là có 2 button có type là submit và cái soup chọn cái sign in with google</v>
-      </c>
-      <c r="F2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Bắt cái cookie cuối cùng
-Chọn đúng button sau</v>
-      </c>
-      <c r="G2" t="str">
-        <v/>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError sqref="A1:H2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tiền xử lý data (chuẩn hóa lương, địa chỉ). Giữ lại tất cả các trường
</commit_message>
<xml_diff>
--- a/docs/Bug/VHung.xlsx
+++ b/docs/Bug/VHung.xlsx
@@ -1,101 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\bigdata\docs\Bug\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E91DB-BF66-4B65-8E9F-26451F7B945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Tác vụ</t>
-  </si>
-  <si>
-    <t>Tác vụ con</t>
-  </si>
-  <si>
-    <t>Hàm/Đối tượng</t>
-  </si>
-  <si>
-    <t>Lỗi/Biểu hiện</t>
-  </si>
-  <si>
-    <t>Nguyên nhân</t>
-  </si>
-  <si>
-    <t>Giải pháp</t>
-  </si>
-  <si>
-    <t>Đã thử</t>
-  </si>
-  <si>
-    <t>Tiến độ</t>
-  </si>
-  <si>
-    <t>Crawl</t>
-  </si>
-  <si>
-    <t>Đăng nhập</t>
-  </si>
-  <si>
-    <t>sign in</t>
-  </si>
-  <si>
-    <t>Không đăng nhập được</t>
-  </si>
-  <si>
-    <t>sau khi nhập tk mk thì nó điều hướng đến trang account.google
-Nguyên nhân rõ hơn là có 2 button có type là submit và cái soup chọn cái sign in with google</t>
-  </si>
-  <si>
-    <t>Bắt cái cookie cuối cùng
-Chọn đúng button sau</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Ngày</t>
-  </si>
-  <si>
-    <t>28/10/2025</t>
-  </si>
-  <si>
-    <t>Tổng thời gian fix</t>
-  </si>
-  <si>
-    <t>4 giờ</t>
-  </si>
-  <si>
-    <t>Kinh nghiệm rút ra</t>
-  </si>
-  <si>
-    <t>Kiểm tra kĩ CSS selector</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -460,86 +396,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Tác vụ</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Tác vụ con</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Hàm/Đối tượng</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Lỗi/Biểu hiện</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Nguyên nhân</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Giải pháp</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Đã thử</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Tiến độ</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Ngày</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Tổng thời gian fix</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Kinh nghiệm rút ra</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
+    <row r="2" xml:space="preserve">
+      <c r="A2" t="str">
+        <v>Crawl</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Đăng nhập</v>
+      </c>
+      <c r="C2" t="str">
+        <v>sign in</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Không đăng nhập được</v>
+      </c>
+      <c r="E2" t="str" xml:space="preserve">
+        <v xml:space="preserve">sau khi nhập tk mk thì nó điều hướng đến trang account.google_x000d_
+Nguyên nhân rõ hơn là có 2 button có type là submit và cái soup chọn cái sign in with google</v>
+      </c>
+      <c r="F2" t="str" xml:space="preserve">
+        <v xml:space="preserve">Bắt cái cookie cuối cùng_x000d_
+Chọn đúng button sau</v>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v>28/10/2025</v>
+      </c>
+      <c r="J2" t="str">
+        <v>4 giờ</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Kiểm tra kĩ CSS selector</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>Preprocess</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Tạo phiên spark</v>
+      </c>
+      <c r="C3" t="str">
+        <v>setup_spark</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Không khởi tạo được</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Không đủ biến môi trường để làm việc</v>
+      </c>
+      <c r="F3" t="str" xml:space="preserve">
+        <v xml:space="preserve">Tải 2 file winutils.exe và hadoop.dll về vào winutils/bin/ và khởi tạo các biến môi trường cần thiết
+Ngoài ra còn cần phải cài đúng phiên bản, ví dụ như pyspark 4.0.1 tải từ pip thì phải đùng hadoop 3.3 (ở đây dùng 3.3.6)</v>
+      </c>
+      <c r="I3" t="str">
+        <v>10/05</v>
+      </c>
+      <c r="J3" t="str">
+        <v>4 giờ</v>
+      </c>
+      <c r="K3" t="str">
+        <v>chịu</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H2" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>